<commit_message>
✨ add NativeAOT and CPP tests
</commit_message>
<xml_diff>
--- a/ParallelPI/Report.xlsx
+++ b/ParallelPI/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hxhon\Documents\CoreCLRUnityBenchmark\ParallelPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2418E9-9507-411D-803C-8E501B7859B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2F0E96-D7EC-4CAE-B8B3-48FC9F1E5E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" xr2:uid="{14517A49-CCC6-414B-A114-DB4274324068}"/>
+    <workbookView xWindow="43425" yWindow="2760" windowWidth="28800" windowHeight="15345" xr2:uid="{14517A49-CCC6-414B-A114-DB4274324068}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,44 +34,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
-  <si>
-    <t>方法</t>
-  </si>
-  <si>
-    <t>总时间(ms)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="25">
   <si>
     <t>每任务时间(μs）</t>
   </si>
   <si>
-    <t>数据组</t>
-  </si>
-  <si>
     <t>MonoJIT</t>
   </si>
   <si>
     <t>任务数</t>
   </si>
   <si>
-    <t>大任务</t>
-  </si>
-  <si>
     <t>Burst</t>
   </si>
   <si>
-    <t>小任务</t>
-  </si>
-  <si>
     <t>Parallel</t>
   </si>
   <si>
     <t>60帧千任务数</t>
   </si>
   <si>
-    <t>中任务</t>
-  </si>
-  <si>
     <t>ParallelFor</t>
   </si>
   <si>
@@ -84,22 +66,49 @@
     <t>Task async</t>
   </si>
   <si>
-    <t>平台</t>
-  </si>
-  <si>
     <t>CoreCLR</t>
   </si>
   <si>
     <t>任务大小</t>
   </si>
   <si>
-    <t>归一化总时间(μs)</t>
-  </si>
-  <si>
-    <t>Parallel No chunk</t>
-  </si>
-  <si>
-    <t>Parallel (Thread local)</t>
+    <t>NativeAOT</t>
+  </si>
+  <si>
+    <t>NativeCPP</t>
+  </si>
+  <si>
+    <t>std::par_unseq</t>
+  </si>
+  <si>
+    <t>ParallelAutoChunk</t>
+  </si>
+  <si>
+    <t>ParallelInline</t>
+  </si>
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>normalized time(μs)</t>
+  </si>
+  <si>
+    <t>totalTime(ms)</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>middle</t>
+  </si>
+  <si>
+    <t>small</t>
   </si>
 </sst>
 </file>
@@ -451,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FA3AF9-4D94-43B5-BBF7-D4C7D4996EB5}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,28 +479,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
         <v>19</v>
@@ -499,71 +508,71 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>65536</v>
+      </c>
+      <c r="C2">
+        <v>65536</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>65536</v>
-      </c>
-      <c r="C2">
-        <v>65536</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2">
-        <f>H2/C2*1000</f>
+        <f t="shared" ref="F2:F32" si="0">H2/C2*1000</f>
         <v>39.489593505859375</v>
       </c>
       <c r="G2">
-        <f>C2/(H2 / 1000)/60/1000</f>
+        <f t="shared" ref="G2:G32" si="1">C2/(H2 / 1000)/60/1000</f>
         <v>0.42205212024260796</v>
       </c>
       <c r="H2">
         <v>2587.9899999999998</v>
       </c>
       <c r="I2">
-        <f>H2/B2*1000</f>
+        <f t="shared" ref="I2:I32" si="2">H2/B2*1000</f>
         <v>39.489593505859375</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>65536</v>
+      </c>
+      <c r="C3">
+        <v>65536</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>65536</v>
-      </c>
-      <c r="C3">
-        <v>65536</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3">
-        <f>H3/C3*1000</f>
+        <f t="shared" si="0"/>
         <v>6.541748046875</v>
       </c>
       <c r="G3">
-        <f>C3/(H3 / 1000)/60/1000</f>
+        <f t="shared" si="1"/>
         <v>2.5477390060334639</v>
       </c>
       <c r="H3">
         <v>428.72</v>
       </c>
       <c r="I3">
-        <f>H3/B3*1000</f>
+        <f t="shared" si="2"/>
         <v>6.541748046875</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>65536</v>
@@ -572,30 +581,30 @@
         <v>65536</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <f>H4/C4*1000</f>
+        <f t="shared" si="0"/>
         <v>39.349365234375</v>
       </c>
       <c r="G4">
-        <f>C4/(H4 / 1000)/60/1000</f>
+        <f t="shared" si="1"/>
         <v>0.42355617599917267</v>
       </c>
       <c r="H4">
         <v>2578.8000000000002</v>
       </c>
       <c r="I4">
-        <f>H4/B4*1000</f>
+        <f t="shared" si="2"/>
         <v>39.349365234375</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>65536</v>
@@ -604,30 +613,30 @@
         <v>65536</v>
       </c>
       <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
       <c r="F5">
-        <f>H5/C5*1000</f>
+        <f t="shared" si="0"/>
         <v>6.665496826171875</v>
       </c>
       <c r="G5">
-        <f>C5/(H5 / 1000)/60/1000</f>
+        <f t="shared" si="1"/>
         <v>2.500438767178689</v>
       </c>
       <c r="H5">
         <v>436.83</v>
       </c>
       <c r="I5">
-        <f>H5/B5*1000</f>
+        <f t="shared" si="2"/>
         <v>6.665496826171875</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>65536</v>
@@ -636,30 +645,30 @@
         <v>65536</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <f>H6/C6*1000</f>
+        <f t="shared" si="0"/>
         <v>6.744384765625</v>
       </c>
       <c r="G6">
-        <f>C6/(H6 / 1000)/60/1000</f>
+        <f t="shared" si="1"/>
         <v>2.4711915535444944</v>
       </c>
       <c r="H6">
         <v>442</v>
       </c>
       <c r="I6">
-        <f>H6/B6*1000</f>
+        <f t="shared" si="2"/>
         <v>6.744384765625</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>65536</v>
@@ -668,30 +677,30 @@
         <v>65536</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F7">
-        <f>H7/C7*1000</f>
+        <f t="shared" si="0"/>
         <v>6.9580078125</v>
       </c>
       <c r="G7">
-        <f>C7/(H7 / 1000)/60/1000</f>
+        <f t="shared" si="1"/>
         <v>2.3953216374269006</v>
       </c>
       <c r="H7">
         <v>456</v>
       </c>
       <c r="I7">
-        <f>H7/B7*1000</f>
+        <f t="shared" si="2"/>
         <v>6.9580078125</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>65536</v>
@@ -700,158 +709,158 @@
         <v>65536</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <f>H8/C8*1000</f>
-        <v>7.080078125</v>
+        <f t="shared" si="0"/>
+        <v>7.8582763671875</v>
       </c>
       <c r="G8">
-        <f>C8/(H8 / 1000)/60/1000</f>
-        <v>2.3540229885057471</v>
+        <f t="shared" si="1"/>
+        <v>2.1209061488673138</v>
       </c>
       <c r="H8">
-        <v>464</v>
+        <v>515</v>
       </c>
       <c r="I8">
-        <f>H8/B8*1000</f>
-        <v>7.080078125</v>
+        <f t="shared" si="2"/>
+        <v>7.8582763671875</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>4096</v>
+        <v>65536</v>
       </c>
       <c r="C9">
         <v>65536</v>
       </c>
       <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
       <c r="F9">
-        <f>H9/C9*1000</f>
-        <v>2.475128173828125</v>
+        <f t="shared" ref="F9:F11" si="3">H9/C9*1000</f>
+        <v>6.481170654296875</v>
       </c>
       <c r="G9">
-        <f>C9/(H9 / 1000)/60/1000</f>
-        <v>6.7336580153299206</v>
+        <f t="shared" ref="G9:G11" si="4">C9/(H9 / 1000)/60/1000</f>
+        <v>2.5715518932705512</v>
       </c>
       <c r="H9">
-        <v>162.21</v>
+        <v>424.75</v>
       </c>
       <c r="I9">
-        <f>H9/B9*1000</f>
-        <v>39.60205078125</v>
+        <f t="shared" ref="I9:I11" si="5">H9/B9*1000</f>
+        <v>6.481170654296875</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>4096</v>
+        <v>65536</v>
       </c>
       <c r="C10">
         <v>65536</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F10">
-        <f>H10/C10*1000</f>
-        <v>0.406646728515625</v>
+        <f t="shared" si="3"/>
+        <v>6.591796875</v>
       </c>
       <c r="G10">
-        <f>C10/(H10 / 1000)/60/1000</f>
-        <v>40.985616010006254</v>
+        <f t="shared" si="4"/>
+        <v>2.528395061728395</v>
       </c>
       <c r="H10">
-        <v>26.65</v>
+        <v>432</v>
       </c>
       <c r="I10">
-        <f>H10/B10*1000</f>
-        <v>6.50634765625</v>
+        <f t="shared" si="5"/>
+        <v>6.591796875</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B11">
-        <v>4096</v>
+        <v>65536</v>
       </c>
       <c r="C11">
         <v>65536</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F11">
-        <f>H11/C11*1000</f>
-        <v>2.801971435546875</v>
+        <f t="shared" si="3"/>
+        <v>7.5702667236328125</v>
       </c>
       <c r="G11">
-        <f>C11/(H11 / 1000)/60/1000</f>
-        <v>5.9481929241772411</v>
+        <f t="shared" si="4"/>
+        <v>2.2015957000083985</v>
       </c>
       <c r="H11">
-        <v>183.63</v>
+        <v>496.125</v>
       </c>
       <c r="I11">
-        <f>H11/B11*1000</f>
-        <v>44.83154296875</v>
+        <f t="shared" si="5"/>
+        <v>7.5702667236328125</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B12">
-        <v>4096</v>
+        <v>65536</v>
       </c>
       <c r="C12">
         <v>65536</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12">
-        <f>H12/C12*1000</f>
-        <v>0.56915283203125</v>
+        <f t="shared" ref="F12" si="6">H12/C12*1000</f>
+        <v>6.683349609375</v>
       </c>
       <c r="G12">
-        <f>C12/(H12 / 1000)/60/1000</f>
-        <v>29.283288650580875</v>
+        <f t="shared" ref="G12" si="7">C12/(H12 / 1000)/60/1000</f>
+        <v>2.4937595129375953</v>
       </c>
       <c r="H12">
-        <v>37.299999999999997</v>
+        <v>438</v>
       </c>
       <c r="I12">
-        <f>H12/B12*1000</f>
-        <v>9.1064453125</v>
+        <f t="shared" ref="I12" si="8">H12/B12*1000</f>
+        <v>6.683349609375</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>4096</v>
@@ -860,30 +869,30 @@
         <v>65536</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F13">
-        <f>H13/C13*1000</f>
-        <v>0.537872314453125</v>
+        <f t="shared" si="0"/>
+        <v>2.475128173828125</v>
       </c>
       <c r="G13">
-        <f>C13/(H13 / 1000)/60/1000</f>
-        <v>30.986288416075652</v>
+        <f t="shared" si="1"/>
+        <v>6.7336580153299206</v>
       </c>
       <c r="H13">
-        <v>35.25</v>
+        <v>162.21</v>
       </c>
       <c r="I13">
-        <f>H13/B13*1000</f>
-        <v>8.60595703125</v>
+        <f t="shared" si="2"/>
+        <v>39.60205078125</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>4096</v>
@@ -892,30 +901,30 @@
         <v>65536</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F14">
-        <f>H14/C14*1000</f>
-        <v>0.568389892578125</v>
+        <f t="shared" si="0"/>
+        <v>0.406646728515625</v>
       </c>
       <c r="G14">
-        <f>C14/(H14 / 1000)/60/1000</f>
-        <v>29.322595078299774</v>
+        <f t="shared" si="1"/>
+        <v>40.985616010006254</v>
       </c>
       <c r="H14">
-        <v>37.25</v>
+        <v>26.65</v>
       </c>
       <c r="I14">
-        <f>H14/B14*1000</f>
-        <v>9.09423828125</v>
+        <f t="shared" si="2"/>
+        <v>6.50634765625</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>4096</v>
@@ -924,30 +933,30 @@
         <v>65536</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F15">
-        <f>H15/C15*1000</f>
-        <v>0.896453857421875</v>
+        <f t="shared" si="0"/>
+        <v>2.801971435546875</v>
       </c>
       <c r="G15">
-        <f>C15/(H15 / 1000)/60/1000</f>
-        <v>18.59177304964539</v>
+        <f t="shared" si="1"/>
+        <v>5.9481929241772411</v>
       </c>
       <c r="H15">
-        <v>58.75</v>
+        <v>183.63</v>
       </c>
       <c r="I15">
-        <f>H15/B15*1000</f>
-        <v>14.34326171875</v>
+        <f t="shared" si="2"/>
+        <v>44.83154296875</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>4096</v>
@@ -956,254 +965,254 @@
         <v>65536</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F16">
-        <f>H16/C16*1000</f>
-        <v>0.476837158203125</v>
+        <f t="shared" si="0"/>
+        <v>0.56915283203125</v>
       </c>
       <c r="G16">
-        <f>C16/(H16 / 1000)/60/1000</f>
-        <v>34.952533333333335</v>
+        <f t="shared" si="1"/>
+        <v>29.283288650580875</v>
       </c>
       <c r="H16">
-        <v>31.25</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I16">
-        <f>H16/B16*1000</f>
-        <v>7.62939453125</v>
+        <f t="shared" si="2"/>
+        <v>9.1064453125</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B17">
-        <v>128</v>
+        <v>4096</v>
       </c>
       <c r="C17">
         <v>65536</v>
       </c>
       <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
       <c r="F17">
-        <f>H17/C17*1000</f>
-        <v>8.1634521484375E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.6046295166015625</v>
       </c>
       <c r="G17">
-        <f>C17/(H17 / 1000)/60/1000</f>
-        <v>204.16199376947043</v>
+        <f t="shared" si="1"/>
+        <v>27.565089379600419</v>
       </c>
       <c r="H17">
-        <v>5.35</v>
+        <v>39.625</v>
       </c>
       <c r="I17">
-        <f>H17/B17*1000</f>
-        <v>41.796875</v>
+        <f t="shared" si="2"/>
+        <v>9.674072265625</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>4096</v>
+      </c>
+      <c r="C18">
+        <v>65536</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="B18">
-        <v>128</v>
-      </c>
-      <c r="C18">
-        <v>65536</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
       <c r="F18">
-        <f>H18/C18*1000</f>
-        <v>1.40380859375E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.720977783203125</v>
       </c>
       <c r="G18">
-        <f>C18/(H18 / 1000)/60/1000</f>
-        <v>1187.2463768115942</v>
+        <f t="shared" si="1"/>
+        <v>23.116754850088185</v>
       </c>
       <c r="H18">
-        <v>0.92</v>
+        <v>47.25</v>
       </c>
       <c r="I18">
-        <f>H18/B18*1000</f>
-        <v>7.1875</v>
+        <f t="shared" si="2"/>
+        <v>11.53564453125</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B19">
-        <v>128</v>
+        <v>4096</v>
       </c>
       <c r="C19">
         <v>65536</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F19">
-        <f>H19/C19*1000</f>
-        <v>0.63232421875</v>
+        <f t="shared" si="0"/>
+        <v>0.7839202880859375</v>
       </c>
       <c r="G19">
-        <f>C19/(H19 / 1000)/60/1000</f>
-        <v>26.357786357786356</v>
+        <f t="shared" si="1"/>
+        <v>21.260665044606654</v>
       </c>
       <c r="H19">
-        <v>41.44</v>
+        <v>51.375</v>
       </c>
       <c r="I19">
-        <f>H19/B19*1000</f>
-        <v>323.75</v>
+        <f t="shared" si="2"/>
+        <v>12.542724609375</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>128</v>
+        <v>4096</v>
       </c>
       <c r="C20">
         <v>65536</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <f>H20/C20*1000</f>
-        <v>0.657958984375</v>
+        <f t="shared" ref="F20:F23" si="9">H20/C20*1000</f>
+        <v>0.4177093505859375</v>
       </c>
       <c r="G20">
-        <f>C20/(H20 / 1000)/60/1000</f>
-        <v>25.330859616573903</v>
+        <f t="shared" si="1"/>
+        <v>39.900152207001526</v>
       </c>
       <c r="H20">
-        <v>43.12</v>
+        <v>27.375</v>
       </c>
       <c r="I20">
-        <f>H20/B20*1000</f>
-        <v>336.875</v>
+        <f t="shared" ref="I20:I23" si="10">H20/B20*1000</f>
+        <v>6.683349609375</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>4096</v>
+      </c>
+      <c r="C21">
+        <v>65536</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
         <v>8</v>
       </c>
-      <c r="B21">
-        <v>128</v>
-      </c>
-      <c r="C21">
-        <v>65536</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
       <c r="F21">
-        <f>H21/C21*1000</f>
-        <v>5.340576171875E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.499725341796875</v>
       </c>
       <c r="G21">
-        <f>C21/(H21 / 1000)/60/1000</f>
-        <v>312.07619047619045</v>
+        <f t="shared" si="1"/>
+        <v>33.351653944020356</v>
       </c>
       <c r="H21">
-        <v>3.5</v>
+        <v>32.75</v>
       </c>
       <c r="I21">
-        <f>H21/B21*1000</f>
-        <v>27.34375</v>
+        <f t="shared" si="10"/>
+        <v>7.99560546875</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B22">
-        <v>128</v>
+        <v>4096</v>
       </c>
       <c r="C22">
         <v>65536</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F22">
-        <f>H22/C22*1000</f>
-        <v>0.37384033203125</v>
+        <f t="shared" si="9"/>
+        <v>0.5779266357421875</v>
       </c>
       <c r="G22">
-        <f>C22/(H22 / 1000)/60/1000</f>
-        <v>44.582312925170065</v>
+        <f t="shared" si="1"/>
+        <v>28.838723872387241</v>
       </c>
       <c r="H22">
-        <v>24.5</v>
+        <v>37.875</v>
       </c>
       <c r="I22">
-        <f>H22/B22*1000</f>
-        <v>191.40625</v>
+        <f t="shared" si="10"/>
+        <v>9.246826171875</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>128</v>
+        <v>4096</v>
       </c>
       <c r="C23">
         <v>65536</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23">
-        <f>H23/C23*1000</f>
-        <v>0.1125335693359375</v>
+        <f t="shared" si="9"/>
+        <v>0.42510986328125</v>
       </c>
       <c r="G23">
-        <f>C23/(H23 / 1000)/60/1000</f>
-        <v>148.10395480225989</v>
+        <f t="shared" si="1"/>
+        <v>39.205551567360615</v>
       </c>
       <c r="H23">
-        <v>7.375</v>
+        <v>27.86</v>
       </c>
       <c r="I23">
-        <f>H23/B23*1000</f>
-        <v>57.6171875</v>
+        <f t="shared" si="10"/>
+        <v>6.8017578125</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>128</v>
@@ -1212,30 +1221,30 @@
         <v>65536</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F24">
-        <f>H24/C24*1000</f>
-        <v>4.1961669921875E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.1634521484375E-2</v>
       </c>
       <c r="G24">
-        <f>C24/(H24 / 1000)/60/1000</f>
-        <v>397.18787878787884</v>
+        <f t="shared" si="1"/>
+        <v>204.16199376947043</v>
       </c>
       <c r="H24">
-        <v>2.75</v>
+        <v>5.35</v>
       </c>
       <c r="I24">
-        <f>H24/B24*1000</f>
-        <v>21.484375</v>
+        <f t="shared" si="2"/>
+        <v>41.796875</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>128</v>
@@ -1244,25 +1253,441 @@
         <v>65536</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F25">
-        <f>H25/C25*1000</f>
-        <v>1.1444091796875E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.40380859375E-2</v>
       </c>
       <c r="G25">
-        <f>C25/(H25 / 1000)/60/1000</f>
-        <v>1456.3555555555556</v>
+        <f t="shared" si="1"/>
+        <v>1187.2463768115942</v>
       </c>
       <c r="H25">
-        <v>0.75</v>
+        <v>0.92</v>
       </c>
       <c r="I25">
-        <f>H25/B25*1000</f>
-        <v>5.859375</v>
+        <f t="shared" si="2"/>
+        <v>7.1875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>128</v>
+      </c>
+      <c r="C26">
+        <v>65536</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.63232421875</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>26.357786357786356</v>
+      </c>
+      <c r="H26">
+        <v>41.44</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>323.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>128</v>
+      </c>
+      <c r="C27">
+        <v>65536</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0.657958984375</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>25.330859616573903</v>
+      </c>
+      <c r="H27">
+        <v>43.12</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>336.875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>128</v>
+      </c>
+      <c r="C28">
+        <v>65536</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>5.340576171875E-2</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>312.07619047619045</v>
+      </c>
+      <c r="H28">
+        <v>3.5</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>27.34375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>128</v>
+      </c>
+      <c r="C29">
+        <v>65536</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0.37384033203125</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>44.582312925170065</v>
+      </c>
+      <c r="H29">
+        <v>24.5</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>191.40625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <v>128</v>
+      </c>
+      <c r="C30">
+        <v>65536</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0.28228759765625</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>59.041441441441442</v>
+      </c>
+      <c r="H30">
+        <v>18.5</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>144.53125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>128</v>
+      </c>
+      <c r="C31">
+        <v>65536</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>1.71661376953125E-2</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>970.90370370370374</v>
+      </c>
+      <c r="H31">
+        <v>1.125</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>8.7890625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <v>128</v>
+      </c>
+      <c r="C32">
+        <v>65536</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1.33514404296875E-2</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>1248.3047619047618</v>
+      </c>
+      <c r="H32">
+        <v>0.875</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>6.8359375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33">
+        <v>128</v>
+      </c>
+      <c r="C33">
+        <v>65536</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33:F37" si="11">H33/C33*1000</f>
+        <v>5.7220458984375E-2</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33:G37" si="12">C33/(H33 / 1000)/60/1000</f>
+        <v>291.27111111111111</v>
+      </c>
+      <c r="H33">
+        <v>3.75</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:I37" si="13">H33/B33*1000</f>
+        <v>29.296875</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <v>128</v>
+      </c>
+      <c r="C34">
+        <v>65536</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="11"/>
+        <v>0.186920166015625</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="12"/>
+        <v>89.16462585034013</v>
+      </c>
+      <c r="H34">
+        <v>12.25</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="13"/>
+        <v>95.703125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>128</v>
+      </c>
+      <c r="C35">
+        <v>65536</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="11"/>
+        <v>0.152587890625</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="12"/>
+        <v>109.22666666666667</v>
+      </c>
+      <c r="H35">
+        <v>10</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="13"/>
+        <v>78.125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
+        <v>128</v>
+      </c>
+      <c r="C36">
+        <v>65536</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="11"/>
+        <v>3.814697265625E-3</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="12"/>
+        <v>4369.0666666666666</v>
+      </c>
+      <c r="H36">
+        <v>0.25</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="13"/>
+        <v>1.953125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <v>128</v>
+      </c>
+      <c r="C37">
+        <v>65536</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="11"/>
+        <v>9.5367431640625E-3</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="12"/>
+        <v>1747.6266666666668</v>
+      </c>
+      <c r="H37">
+        <v>0.625</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="13"/>
+        <v>4.8828125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>128</v>
+      </c>
+      <c r="C38">
+        <v>65536</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38">
+        <f t="shared" ref="F38" si="14">H38/C38*1000</f>
+        <v>4.034423828125E-2</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38" si="15">C38/(H38 / 1000)/60/1000</f>
+        <v>413.11144730206757</v>
+      </c>
+      <c r="H38">
+        <v>2.6440000000000001</v>
+      </c>
+      <c r="I38">
+        <f t="shared" ref="I38" si="16">H38/B38*1000</f>
+        <v>20.65625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>